<commit_message>
Ocr app ,second commit
</commit_message>
<xml_diff>
--- a/media/excel/ocr-result.xlsx
+++ b/media/excel/ocr-result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,30 +649,25 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>\4,</t>
+          <t>\4,968</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>968</t>
+          <t>注文者</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>注文者</t>
+          <t>:</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>:</t>
+          <t>次材・購買課</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
-        <is>
-          <t>次材・購買課</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
         <is>
           <t>工藤</t>
         </is>
@@ -769,7 +764,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Plate</t>
+          <t>Pate</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -799,35 +794,30 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>\1,</t>
+          <t>\1,200|</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>200|</t>
+          <t>9月10日</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>9月10日</t>
+          <t>|</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>池田</t>
+          <t>|9/5ヤグチ精機様持込み</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ精機様持込み</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
         <is>
           <t>間</t>
         </is>
@@ -844,7 +834,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Plate</t>
+          <t>Pate</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -874,7 +864,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>\],200|</t>
+          <t>\1,200|</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -914,7 +904,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Plate</t>
+          <t>Pate</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -944,35 +934,30 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>\1,</t>
+          <t>\1,200|</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>200|</t>
+          <t>9月10日</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>9月10日</t>
+          <t>|</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>池田</t>
+          <t>|9/5ヤグチ精機様持込み</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ精機様持込み</t>
-        </is>
-      </c>
-      <c r="O17" t="inlineStr">
         <is>
           <t>拓</t>
         </is>
@@ -989,7 +974,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Plate</t>
+          <t>Pate</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">

</xml_diff>

<commit_message>
Ocr app ,third commit
</commit_message>
<xml_diff>
--- a/media/excel/ocr-result.xlsx
+++ b/media/excel/ocr-result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,7 +719,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>数量|</t>
+          <t>数量</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -734,7 +734,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>|希望納期|</t>
+          <t>希望納期</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>\1,200|</t>
+          <t>\1,200</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -804,20 +804,15 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>池田</t>
+          <t>9/5ヤグチ精機様持込み</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ精機様持込み</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
         <is>
           <t>間</t>
         </is>
@@ -864,7 +859,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>\1,200|</t>
+          <t>\1,200</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -874,20 +869,15 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>池田</t>
+          <t>9/5ヤグチ精機様持込み</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ精機様持込み</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
         <is>
           <t>に</t>
         </is>
@@ -934,7 +924,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>\1,200|</t>
+          <t>\1,200</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -944,20 +934,15 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>池田</t>
+          <t>9/5ヤグチ精機様持込み</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ精機様持込み</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
         <is>
           <t>拓</t>
         </is>
@@ -1004,7 +989,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>\1,000|</t>
+          <t>\1,000</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1014,17 +999,12 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>|</t>
+          <t>池田</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>池田</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>|9/5ヤグチ糖機様持込み</t>
+          <t>9/5ヤグチ糖機様持込み</t>
         </is>
       </c>
     </row>
@@ -1052,46 +1032,16 @@
       <c r="A20" t="n">
         <v>17</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>18</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>19</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1154,11 +1104,6 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
           <t>\368</t>
         </is>
       </c>
@@ -1188,16 +1133,6 @@
         </is>
       </c>
       <c r="F26" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>|</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
         <is>
           <t>\4、968</t>
         </is>

</xml_diff>